<commit_message>
Update processing multiple form in Mentawai.
</commit_message>
<xml_diff>
--- a/C-grp-04-HolleList-01_28385_assignsubmission_file/Mentawai/Mentawai-notes-and-additional data.xlsx
+++ b/C-grp-04-HolleList-01_28385_assignsubmission_file/Mentawai/Mentawai-notes-and-additional data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Primahadi/Documents/research/Lexiology_Lexicography_Even-2024_Holle_List_Barrier_Islands/C-grp-04-HolleList-01_28385_assignsubmission_file/Mentawai/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC40D95-7EB0-5547-B3AA-8A90C61D8702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6917F1-6927-E94F-9633-13B193CD65FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14480" yWindow="660" windowWidth="14180" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>WORD/EXPRESSION</t>
   </si>
@@ -286,9 +286,6 @@
     <t>to go ashore</t>
   </si>
   <si>
-    <t>bakatkoe - sita, sibakat nia, kai sibakat nia bakat</t>
-  </si>
-  <si>
     <t>possession</t>
   </si>
   <si>
@@ -526,12 +523,6 @@
     <t>toedjôlou</t>
   </si>
   <si>
-    <t>&lt;he&gt; who is the hindmost</t>
-  </si>
-  <si>
-    <t>oen , oek</t>
-  </si>
-  <si>
     <t>bakat</t>
   </si>
   <si>
@@ -546,16 +537,29 @@
   <si>
     <t>also 'up to that point'</t>
   </si>
+  <si>
+    <t>bakatkoe - sita, sibakat nia, kai sibakat nia</t>
+  </si>
+  <si>
+    <t>&lt;he&gt; who is the hindmost (oen , oek)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -612,14 +616,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,8 +846,8 @@
   <dimension ref="A1:Z1008"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C99" sqref="C99"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -935,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -966,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1126,7 +1131,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -1194,13 +1199,13 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="1">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1334,7 +1339,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1398,7 +1403,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1426,7 +1431,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="1">
         <v>10</v>
@@ -1528,7 +1533,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="1">
         <v>11</v>
@@ -1864,7 +1869,7 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B31" s="1">
         <v>17</v>
@@ -1902,7 +1907,7 @@
         <v>18</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1930,13 +1935,13 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B33" s="1">
         <v>19</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1998,13 +2003,13 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="1">
         <v>21</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -2196,13 +2201,13 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="1">
         <v>25</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2230,13 +2235,13 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" s="1">
         <v>25</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -2264,7 +2269,7 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B43" s="1">
         <v>26</v>
@@ -2296,13 +2301,13 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B44" s="1">
         <v>27</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2330,13 +2335,13 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B45" s="1">
         <v>28</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -2364,13 +2369,13 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B46" s="1">
         <v>28</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -2528,13 +2533,13 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B51" s="1">
         <v>32</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -2562,13 +2567,13 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B52" s="1">
         <v>32</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -2596,14 +2601,14 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B53" s="1">
         <v>33</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2630,7 +2635,7 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B54" s="1">
         <v>34</v>
@@ -2662,13 +2667,13 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B55" s="1">
         <v>35</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -2696,13 +2701,13 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B56" s="1">
         <v>35</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2730,13 +2735,13 @@
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" s="1">
         <v>35</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -2764,13 +2769,13 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B58" s="1">
         <v>35</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -2798,7 +2803,7 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B59" s="1">
         <v>36</v>
@@ -2870,7 +2875,7 @@
         <v>38</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -2898,13 +2903,13 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B62" s="1">
         <v>39</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2932,13 +2937,13 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B63" s="1">
         <v>39</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -2966,13 +2971,13 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B64" s="1">
         <v>39</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -3000,13 +3005,13 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B65" s="1">
         <v>40</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -3034,13 +3039,13 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B66" s="1">
         <v>40</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -3068,7 +3073,7 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B67" s="1">
         <v>40</v>
@@ -3100,13 +3105,13 @@
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B68" s="1">
         <v>41</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -3168,13 +3173,13 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B70" s="1">
         <v>42</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -3234,13 +3239,13 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B72" s="1">
         <v>44</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -3268,13 +3273,13 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B73" s="1">
         <v>44</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -3302,13 +3307,13 @@
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B74" s="1">
         <v>45</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -3342,7 +3347,7 @@
         <v>45</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -3374,7 +3379,7 @@
         <v>46</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -3606,7 +3611,7 @@
         <v>51</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -3637,7 +3642,7 @@
         <v>52</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -3771,7 +3776,7 @@
         <v>55</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -3805,7 +3810,7 @@
         <v>56</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -3833,7 +3838,7 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B90" s="1">
         <v>56</v>
@@ -3866,14 +3871,12 @@
       <c r="Z90" s="1"/>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>169</v>
-      </c>
+      <c r="A91" s="3"/>
       <c r="B91" s="1">
         <v>57</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>168</v>
+      <c r="C91" s="5" t="s">
+        <v>173</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -3900,8 +3903,8 @@
       <c r="Z91" s="1"/>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>88</v>
+      <c r="A92" s="5" t="s">
+        <v>172</v>
       </c>
       <c r="B92" s="1">
         <v>58</v>
@@ -3933,13 +3936,13 @@
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B93" s="1">
         <v>58</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -3967,13 +3970,13 @@
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B94" s="1">
         <v>59</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -4001,13 +4004,13 @@
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B95" s="1">
         <v>60</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -4035,13 +4038,13 @@
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B96" s="1">
         <v>60</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -4069,13 +4072,13 @@
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B97" s="1">
         <v>61</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -4103,13 +4106,13 @@
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B98" s="1">
         <v>61</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -4140,7 +4143,7 @@
         <v>62</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>

</xml_diff>